<commit_message>
add gender cat and gen positions to race results
</commit_message>
<xml_diff>
--- a/results/Bx5.xlsx
+++ b/results/Bx5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sx5standings\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344F8191-8F0C-4E86-91A3-BCB21DC28219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA14664A-979B-49EB-9307-51BF288D1021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="238">
   <si>
     <t>Forename</t>
   </si>
@@ -2333,6 +2333,9 @@
   </si>
   <si>
     <t>ResultAsText</t>
+  </si>
+  <si>
+    <t>Gender</t>
   </si>
 </sst>
 </file>
@@ -2810,7 +2813,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
@@ -2829,7 +2832,7 @@
     <col min="10" max="10" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2860,8 +2863,11 @@
       <c r="J1" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -2891,8 +2897,12 @@
         <f>TEXT(F2,"hh:mm:ss")</f>
         <v>00:17:42</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" t="str">
+        <f>IF(LEFT(D2,1)="M","M","F")</f>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
@@ -2922,8 +2932,12 @@
         <f t="shared" ref="J3:J66" si="0">TEXT(F3,"hh:mm:ss")</f>
         <v>00:17:49</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K66" si="1">IF(LEFT(D3,1)="M","M","F")</f>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -2953,8 +2967,12 @@
         <f t="shared" si="0"/>
         <v>00:17:54</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -2986,8 +3004,12 @@
         <f t="shared" si="0"/>
         <v>00:18:36</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -3017,8 +3039,12 @@
         <f t="shared" si="0"/>
         <v>00:18:50</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -3050,8 +3076,12 @@
         <f t="shared" si="0"/>
         <v>00:18:59</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
@@ -3083,8 +3113,12 @@
         <f t="shared" si="0"/>
         <v>00:19:00</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>27</v>
       </c>
@@ -3116,8 +3150,12 @@
         <f t="shared" si="0"/>
         <v>00:19:40</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -3147,8 +3185,12 @@
         <f t="shared" si="0"/>
         <v>00:19:46</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
@@ -3178,8 +3220,12 @@
         <f t="shared" si="0"/>
         <v>00:20:03</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
@@ -3209,8 +3255,12 @@
         <f t="shared" si="0"/>
         <v>00:20:07</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>37</v>
       </c>
@@ -3242,8 +3292,12 @@
         <f t="shared" si="0"/>
         <v>00:20:20</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>40</v>
       </c>
@@ -3273,8 +3327,12 @@
         <f t="shared" si="0"/>
         <v>00:20:33</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>42</v>
       </c>
@@ -3304,8 +3362,12 @@
         <f t="shared" si="0"/>
         <v>00:20:45</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>44</v>
       </c>
@@ -3337,8 +3399,12 @@
         <f t="shared" si="0"/>
         <v>00:20:58</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>48</v>
       </c>
@@ -3370,8 +3436,12 @@
         <f t="shared" si="0"/>
         <v>00:21:07</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>51</v>
       </c>
@@ -3403,8 +3473,12 @@
         <f t="shared" si="0"/>
         <v>00:21:39</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>54</v>
       </c>
@@ -3436,8 +3510,12 @@
         <f t="shared" si="0"/>
         <v>00:21:48</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>57</v>
       </c>
@@ -3467,8 +3545,12 @@
         <f t="shared" si="0"/>
         <v>00:21:54</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
@@ -3500,8 +3582,12 @@
         <f t="shared" si="0"/>
         <v>00:21:55</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>62</v>
       </c>
@@ -3531,8 +3617,12 @@
         <f t="shared" si="0"/>
         <v>00:21:56</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>63</v>
       </c>
@@ -3564,8 +3654,12 @@
         <f t="shared" si="0"/>
         <v>00:21:59</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>66</v>
       </c>
@@ -3595,8 +3689,12 @@
         <f t="shared" si="0"/>
         <v>00:22:12</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>68</v>
       </c>
@@ -3626,8 +3724,12 @@
         <f t="shared" si="0"/>
         <v>00:22:13</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>70</v>
       </c>
@@ -3659,8 +3761,12 @@
         <f t="shared" si="0"/>
         <v>00:22:27</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>71</v>
       </c>
@@ -3690,8 +3796,12 @@
         <f t="shared" si="0"/>
         <v>00:22:46</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>73</v>
       </c>
@@ -3723,8 +3833,12 @@
         <f t="shared" si="0"/>
         <v>00:22:50</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>76</v>
       </c>
@@ -3754,8 +3868,12 @@
         <f t="shared" si="0"/>
         <v>00:22:51</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>78</v>
       </c>
@@ -3787,8 +3905,12 @@
         <f t="shared" si="0"/>
         <v>00:23:06</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>54</v>
       </c>
@@ -3820,8 +3942,12 @@
         <f t="shared" si="0"/>
         <v>00:23:09</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>82</v>
       </c>
@@ -3851,8 +3977,12 @@
         <f t="shared" si="0"/>
         <v>00:23:13</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>85</v>
       </c>
@@ -3882,8 +4012,12 @@
         <f t="shared" si="0"/>
         <v>00:23:16</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>86</v>
       </c>
@@ -3915,8 +4049,12 @@
         <f t="shared" si="0"/>
         <v>00:23:28</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>70</v>
       </c>
@@ -3946,8 +4084,12 @@
         <f t="shared" si="0"/>
         <v>00:23:31</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>89</v>
       </c>
@@ -3979,8 +4121,12 @@
         <f t="shared" si="0"/>
         <v>00:23:36</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>92</v>
       </c>
@@ -4010,8 +4156,12 @@
         <f t="shared" si="0"/>
         <v>00:23:43</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>94</v>
       </c>
@@ -4041,8 +4191,12 @@
         <f t="shared" si="0"/>
         <v>00:23:48</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K38" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>96</v>
       </c>
@@ -4072,8 +4226,12 @@
         <f t="shared" si="0"/>
         <v>00:23:52</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>98</v>
       </c>
@@ -4105,8 +4263,12 @@
         <f t="shared" si="0"/>
         <v>00:24:00</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K40" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>101</v>
       </c>
@@ -4136,8 +4298,12 @@
         <f t="shared" si="0"/>
         <v>00:24:33</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K41" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>103</v>
       </c>
@@ -4167,8 +4333,12 @@
         <f t="shared" si="0"/>
         <v>00:24:33</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K42" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>105</v>
       </c>
@@ -4198,8 +4368,12 @@
         <f t="shared" si="0"/>
         <v>00:24:38</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K43" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>107</v>
       </c>
@@ -4231,8 +4405,12 @@
         <f t="shared" si="0"/>
         <v>00:24:54</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>109</v>
       </c>
@@ -4262,8 +4440,12 @@
         <f t="shared" si="0"/>
         <v>00:25:10</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K45" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>111</v>
       </c>
@@ -4293,8 +4475,12 @@
         <f t="shared" si="0"/>
         <v>00:25:18</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K46" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>112</v>
       </c>
@@ -4326,8 +4512,12 @@
         <f t="shared" si="0"/>
         <v>00:25:22</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K47" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>25</v>
       </c>
@@ -4357,8 +4547,12 @@
         <f t="shared" si="0"/>
         <v>00:25:23</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K48" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>116</v>
       </c>
@@ -4388,8 +4582,12 @@
         <f t="shared" si="0"/>
         <v>00:25:25</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K49" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>117</v>
       </c>
@@ -4419,8 +4617,12 @@
         <f t="shared" si="0"/>
         <v>00:25:28</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K50" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>119</v>
       </c>
@@ -4452,8 +4654,12 @@
         <f t="shared" si="0"/>
         <v>00:25:41</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K51" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>122</v>
       </c>
@@ -4483,8 +4689,12 @@
         <f t="shared" si="0"/>
         <v>00:25:42</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K52" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>124</v>
       </c>
@@ -4514,8 +4724,12 @@
         <f t="shared" si="0"/>
         <v>00:25:46</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K53" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>126</v>
       </c>
@@ -4545,8 +4759,12 @@
         <f t="shared" si="0"/>
         <v>00:25:51</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K54" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>128</v>
       </c>
@@ -4576,8 +4794,12 @@
         <f t="shared" si="0"/>
         <v>00:25:55</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K55" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>130</v>
       </c>
@@ -4609,8 +4831,12 @@
         <f t="shared" si="0"/>
         <v>00:26:01</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K56" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>132</v>
       </c>
@@ -4642,8 +4868,12 @@
         <f t="shared" si="0"/>
         <v>00:26:06</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K57" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>135</v>
       </c>
@@ -4675,8 +4905,12 @@
         <f t="shared" si="0"/>
         <v>00:26:07</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K58" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>137</v>
       </c>
@@ -4706,8 +4940,12 @@
         <f t="shared" si="0"/>
         <v>00:26:08</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K59" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>139</v>
       </c>
@@ -4737,8 +4975,12 @@
         <f t="shared" si="0"/>
         <v>00:26:11</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K60" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>137</v>
       </c>
@@ -4770,8 +5012,12 @@
         <f t="shared" si="0"/>
         <v>00:26:21</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K61" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>142</v>
       </c>
@@ -4803,8 +5049,12 @@
         <f t="shared" si="0"/>
         <v>00:26:39</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K62" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>145</v>
       </c>
@@ -4834,8 +5084,12 @@
         <f t="shared" si="0"/>
         <v>00:26:41</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K63" t="str">
+        <f t="shared" si="1"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>147</v>
       </c>
@@ -4867,8 +5121,12 @@
         <f t="shared" si="0"/>
         <v>00:26:54</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K64" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>149</v>
       </c>
@@ -4898,8 +5156,12 @@
         <f t="shared" si="0"/>
         <v>00:26:59</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K65" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>151</v>
       </c>
@@ -4929,8 +5191,12 @@
         <f t="shared" si="0"/>
         <v>00:26:59</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K66" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>153</v>
       </c>
@@ -4959,11 +5225,15 @@
         <v>16</v>
       </c>
       <c r="J67" s="13" t="str">
-        <f t="shared" ref="J67:J111" si="1">TEXT(F67,"hh:mm:ss")</f>
+        <f t="shared" ref="J67:J111" si="2">TEXT(F67,"hh:mm:ss")</f>
         <v>00:27:14</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K111" si="3">IF(LEFT(D67,1)="M","M","F")</f>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>155</v>
       </c>
@@ -4992,11 +5262,15 @@
         <v>14</v>
       </c>
       <c r="J68" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:27:18</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K68" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>157</v>
       </c>
@@ -5025,11 +5299,15 @@
         <v>6</v>
       </c>
       <c r="J69" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:27:22</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K69" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>159</v>
       </c>
@@ -5056,11 +5334,15 @@
         <v>7</v>
       </c>
       <c r="J70" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:27:26</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K70" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>161</v>
       </c>
@@ -5089,11 +5371,15 @@
         <v>4</v>
       </c>
       <c r="J71" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:27:33</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K71" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>59</v>
       </c>
@@ -5120,11 +5406,15 @@
         <v>17</v>
       </c>
       <c r="J72" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:27:39</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K72" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>164</v>
       </c>
@@ -5151,11 +5441,15 @@
         <v>7</v>
       </c>
       <c r="J73" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:27:40</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K73" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>166</v>
       </c>
@@ -5184,11 +5478,15 @@
         <v>15</v>
       </c>
       <c r="J74" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:27:42</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K74" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>105</v>
       </c>
@@ -5217,11 +5515,15 @@
         <v>18</v>
       </c>
       <c r="J75" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:27:43</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K75" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>169</v>
       </c>
@@ -5248,11 +5550,15 @@
         <v>8</v>
       </c>
       <c r="J76" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:27:46</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K76" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>170</v>
       </c>
@@ -5279,11 +5585,15 @@
         <v>9</v>
       </c>
       <c r="J77" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:27:49</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K77" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>112</v>
       </c>
@@ -5310,11 +5620,15 @@
         <v>8</v>
       </c>
       <c r="J78" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:28:05</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K78" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>173</v>
       </c>
@@ -5341,11 +5655,15 @@
         <v>10</v>
       </c>
       <c r="J79" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:28:26</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K79" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>175</v>
       </c>
@@ -5372,11 +5690,15 @@
         <v>11</v>
       </c>
       <c r="J80" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:28:45</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K80" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>177</v>
       </c>
@@ -5405,11 +5727,15 @@
         <v>12</v>
       </c>
       <c r="J81" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:28:48</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K81" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>180</v>
       </c>
@@ -5436,11 +5762,15 @@
         <v>1</v>
       </c>
       <c r="J82" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:28:57</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K82" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>183</v>
       </c>
@@ -5467,11 +5797,15 @@
         <v>13</v>
       </c>
       <c r="J83" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:02</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K83" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>185</v>
       </c>
@@ -5500,11 +5834,15 @@
         <v>9</v>
       </c>
       <c r="J84" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:03</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K84" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>187</v>
       </c>
@@ -5533,11 +5871,15 @@
         <v>2</v>
       </c>
       <c r="J85" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:05</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K85" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>189</v>
       </c>
@@ -5566,11 +5908,15 @@
         <v>16</v>
       </c>
       <c r="J86" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:05</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K86" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>191</v>
       </c>
@@ -5599,11 +5945,15 @@
         <v>10</v>
       </c>
       <c r="J87" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:06</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K87" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>9</v>
       </c>
@@ -5632,11 +5982,15 @@
         <v>9</v>
       </c>
       <c r="J88" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:07</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K88" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>111</v>
       </c>
@@ -5665,11 +6019,15 @@
         <v>11</v>
       </c>
       <c r="J89" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:12</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K89" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>196</v>
       </c>
@@ -5698,11 +6056,15 @@
         <v>5</v>
       </c>
       <c r="J90" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:19</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K90" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>198</v>
       </c>
@@ -5731,11 +6093,15 @@
         <v>16</v>
       </c>
       <c r="J91" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:27</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K91" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>200</v>
       </c>
@@ -5762,11 +6128,15 @@
         <v>10</v>
       </c>
       <c r="J92" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:37</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K92" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>202</v>
       </c>
@@ -5795,11 +6165,15 @@
         <v>12</v>
       </c>
       <c r="J93" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:39</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K93" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>203</v>
       </c>
@@ -5828,11 +6202,15 @@
         <v>13</v>
       </c>
       <c r="J94" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:46</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K94" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>205</v>
       </c>
@@ -5859,11 +6237,15 @@
         <v>14</v>
       </c>
       <c r="J95" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:29:54</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K95" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>207</v>
       </c>
@@ -5890,11 +6272,15 @@
         <v>3</v>
       </c>
       <c r="J96" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:30:28</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K96" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>209</v>
       </c>
@@ -5923,11 +6309,15 @@
         <v>6</v>
       </c>
       <c r="J97" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:31:12</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K97" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>211</v>
       </c>
@@ -5954,11 +6344,15 @@
         <v>15</v>
       </c>
       <c r="J98" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:31:24</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K98" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>213</v>
       </c>
@@ -5987,11 +6381,15 @@
         <v>14</v>
       </c>
       <c r="J99" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:31:30</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K99" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>173</v>
       </c>
@@ -6020,11 +6418,15 @@
         <v>17</v>
       </c>
       <c r="J100" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:31:42</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K100" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>59</v>
       </c>
@@ -6053,11 +6455,15 @@
         <v>11</v>
       </c>
       <c r="J101" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:32:32</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K101" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>217</v>
       </c>
@@ -6084,11 +6490,15 @@
         <v>4</v>
       </c>
       <c r="J102" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:32:55</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K102" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>219</v>
       </c>
@@ -6115,11 +6525,15 @@
         <v>15</v>
       </c>
       <c r="J103" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:33:15</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K103" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>221</v>
       </c>
@@ -6146,11 +6560,15 @@
         <v>16</v>
       </c>
       <c r="J104" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:33:58</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K104" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>223</v>
       </c>
@@ -6177,11 +6595,15 @@
         <v>1</v>
       </c>
       <c r="J105" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:34:00</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K105" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>226</v>
       </c>
@@ -6208,11 +6630,15 @@
         <v>17</v>
       </c>
       <c r="J106" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:34:02</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K106" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>227</v>
       </c>
@@ -6239,11 +6665,15 @@
         <v>5</v>
       </c>
       <c r="J107" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:34:08</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K107" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>229</v>
       </c>
@@ -6272,11 +6702,15 @@
         <v>16</v>
       </c>
       <c r="J108" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:34:59</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K108" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>232</v>
       </c>
@@ -6305,11 +6739,15 @@
         <v>19</v>
       </c>
       <c r="J109" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:35:00</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K109" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>233</v>
       </c>
@@ -6336,11 +6774,15 @@
         <v>18</v>
       </c>
       <c r="J110" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:36:44</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K110" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>44</v>
       </c>
@@ -6369,8 +6811,12 @@
         <v>20</v>
       </c>
       <c r="J111" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00:36:45</v>
+      </c>
+      <c r="K111" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simplify recalculate race results function
</commit_message>
<xml_diff>
--- a/results/Bx5.xlsx
+++ b/results/Bx5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sx5standings\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA14664A-979B-49EB-9307-51BF288D1021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D980B29-14FF-4BBF-B78B-C6B69EE2E23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,18 +50,9 @@
     <t>No.</t>
   </si>
   <si>
-    <t>Bx5</t>
-  </si>
-  <si>
     <t>Pos</t>
   </si>
   <si>
-    <t>Gen Pos</t>
-  </si>
-  <si>
-    <t>Cat Pos</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -2336,6 +2327,15 @@
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>GenPos</t>
+  </si>
+  <si>
+    <t>CatPos</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -2816,7 +2816,7 @@
   <dimension ref="A1:K111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2849,34 +2849,34 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>7</v>
+        <v>235</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>8</v>
+        <v>236</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1">
         <v>624</v>
@@ -2904,14 +2904,14 @@
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1">
         <v>652</v>
@@ -2939,14 +2939,14 @@
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1">
         <v>577</v>
@@ -2974,16 +2974,16 @@
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="E5" s="1">
         <v>549</v>
@@ -3011,14 +3011,14 @@
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1">
         <v>567</v>
@@ -3046,16 +3046,16 @@
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
         <v>674</v>
@@ -3083,16 +3083,16 @@
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1">
         <v>569</v>
@@ -3120,16 +3120,16 @@
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1">
         <v>584</v>
@@ -3157,14 +3157,14 @@
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1">
         <v>585</v>
@@ -3192,14 +3192,14 @@
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1">
         <v>682</v>
@@ -3227,14 +3227,14 @@
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1">
         <v>598</v>
@@ -3262,16 +3262,16 @@
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1">
         <v>635</v>
@@ -3299,14 +3299,14 @@
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1">
         <v>611</v>
@@ -3334,14 +3334,14 @@
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1">
         <v>657</v>
@@ -3369,16 +3369,16 @@
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="E16" s="1">
         <v>661</v>
@@ -3406,16 +3406,16 @@
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1">
         <v>73</v>
@@ -3443,16 +3443,16 @@
     </row>
     <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E18" s="1">
         <v>654</v>
@@ -3480,16 +3480,16 @@
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E19" s="1">
         <v>656</v>
@@ -3517,14 +3517,14 @@
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E20" s="1">
         <v>641</v>
@@ -3552,16 +3552,16 @@
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21" s="1">
         <v>137</v>
@@ -3589,14 +3589,14 @@
     </row>
     <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E22" s="1">
         <v>683</v>
@@ -3624,16 +3624,16 @@
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E23" s="1">
         <v>571</v>
@@ -3661,14 +3661,14 @@
     </row>
     <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E24" s="1">
         <v>625</v>
@@ -3696,14 +3696,14 @@
     </row>
     <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E25" s="1">
         <v>579</v>
@@ -3731,16 +3731,16 @@
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E26" s="1">
         <v>555</v>
@@ -3768,14 +3768,14 @@
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E27" s="1">
         <v>556</v>
@@ -3803,16 +3803,16 @@
     </row>
     <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E28" s="1">
         <v>559</v>
@@ -3840,14 +3840,14 @@
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1">
         <v>644</v>
@@ -3875,16 +3875,16 @@
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E30" s="1">
         <v>96</v>
@@ -3912,16 +3912,16 @@
     </row>
     <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E31" s="1">
         <v>604</v>
@@ -3949,14 +3949,14 @@
     </row>
     <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E32" s="1">
         <v>680</v>
@@ -3984,14 +3984,14 @@
     </row>
     <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E33" s="1">
         <v>599</v>
@@ -4019,16 +4019,16 @@
     </row>
     <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E34" s="1">
         <v>560</v>
@@ -4056,14 +4056,14 @@
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1">
         <v>626</v>
@@ -4091,16 +4091,16 @@
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E36" s="1">
         <v>574</v>
@@ -4128,14 +4128,14 @@
     </row>
     <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E37" s="1">
         <v>642</v>
@@ -4163,14 +4163,14 @@
     </row>
     <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E38" s="1">
         <v>692</v>
@@ -4198,14 +4198,14 @@
     </row>
     <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E39" s="1">
         <v>126</v>
@@ -4233,16 +4233,16 @@
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E40" s="1">
         <v>655</v>
@@ -4270,14 +4270,14 @@
     </row>
     <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E41" s="1">
         <v>63</v>
@@ -4305,14 +4305,14 @@
     </row>
     <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E42" s="1">
         <v>573</v>
@@ -4340,14 +4340,14 @@
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E43" s="1">
         <v>591</v>
@@ -4375,16 +4375,16 @@
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E44" s="1">
         <v>678</v>
@@ -4412,14 +4412,14 @@
     </row>
     <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E45" s="1">
         <v>691</v>
@@ -4447,14 +4447,14 @@
     </row>
     <row r="46" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E46" s="1">
         <v>684</v>
@@ -4482,16 +4482,16 @@
     </row>
     <row r="47" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E47" s="1">
         <v>72</v>
@@ -4519,14 +4519,14 @@
     </row>
     <row r="48" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E48" s="1">
         <v>562</v>
@@ -4554,14 +4554,14 @@
     </row>
     <row r="49" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C49" s="11"/>
       <c r="D49" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E49" s="1">
         <v>578</v>
@@ -4589,14 +4589,14 @@
     </row>
     <row r="50" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E50" s="1">
         <v>663</v>
@@ -4624,16 +4624,16 @@
     </row>
     <row r="51" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E51" s="1">
         <v>619</v>
@@ -4661,14 +4661,14 @@
     </row>
     <row r="52" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E52" s="1">
         <v>636</v>
@@ -4696,14 +4696,14 @@
     </row>
     <row r="53" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C53" s="11"/>
       <c r="D53" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E53" s="1">
         <v>615</v>
@@ -4731,14 +4731,14 @@
     </row>
     <row r="54" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E54" s="1">
         <v>688</v>
@@ -4766,14 +4766,14 @@
     </row>
     <row r="55" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C55" s="11"/>
       <c r="D55" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E55" s="1">
         <v>612</v>
@@ -4801,16 +4801,16 @@
     </row>
     <row r="56" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E56" s="1">
         <v>639</v>
@@ -4838,16 +4838,16 @@
     </row>
     <row r="57" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E57" s="1">
         <v>548</v>
@@ -4875,16 +4875,16 @@
     </row>
     <row r="58" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E58" s="1">
         <v>632</v>
@@ -4912,14 +4912,14 @@
     </row>
     <row r="59" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E59" s="1">
         <v>128</v>
@@ -4947,14 +4947,14 @@
     </row>
     <row r="60" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E60" s="1">
         <v>575</v>
@@ -4982,16 +4982,16 @@
     </row>
     <row r="61" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E61" s="1">
         <v>638</v>
@@ -5019,16 +5019,16 @@
     </row>
     <row r="62" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E62" s="1">
         <v>659</v>
@@ -5056,14 +5056,14 @@
     </row>
     <row r="63" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E63" s="1">
         <v>648</v>
@@ -5091,16 +5091,16 @@
     </row>
     <row r="64" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E64" s="1">
         <v>634</v>
@@ -5128,14 +5128,14 @@
     </row>
     <row r="65" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C65" s="11"/>
       <c r="D65" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E65" s="1">
         <v>610</v>
@@ -5163,14 +5163,14 @@
     </row>
     <row r="66" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C66" s="11"/>
       <c r="D66" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E66" s="1">
         <v>672</v>
@@ -5198,16 +5198,16 @@
     </row>
     <row r="67" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E67" s="1">
         <v>633</v>
@@ -5235,16 +5235,16 @@
     </row>
     <row r="68" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E68" s="1">
         <v>637</v>
@@ -5272,16 +5272,16 @@
     </row>
     <row r="69" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E69" s="1">
         <v>690</v>
@@ -5309,14 +5309,14 @@
     </row>
     <row r="70" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C70" s="12"/>
       <c r="D70" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E70" s="1">
         <v>59</v>
@@ -5344,16 +5344,16 @@
     </row>
     <row r="71" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E71" s="1">
         <v>669</v>
@@ -5381,14 +5381,14 @@
     </row>
     <row r="72" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E72" s="1">
         <v>676</v>
@@ -5416,14 +5416,14 @@
     </row>
     <row r="73" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E73" s="1">
         <v>677</v>
@@ -5451,16 +5451,16 @@
     </row>
     <row r="74" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E74" s="1">
         <v>582</v>
@@ -5488,16 +5488,16 @@
     </row>
     <row r="75" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E75" s="1">
         <v>583</v>
@@ -5525,14 +5525,14 @@
     </row>
     <row r="76" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E76" s="1">
         <v>590</v>
@@ -5560,14 +5560,14 @@
     </row>
     <row r="77" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E77" s="1">
         <v>685</v>
@@ -5595,14 +5595,14 @@
     </row>
     <row r="78" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E78" s="1">
         <v>679</v>
@@ -5630,14 +5630,14 @@
     </row>
     <row r="79" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E79" s="1">
         <v>613</v>
@@ -5665,14 +5665,14 @@
     </row>
     <row r="80" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E80" s="1">
         <v>609</v>
@@ -5700,16 +5700,16 @@
     </row>
     <row r="81" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E81" s="1">
         <v>645</v>
@@ -5737,14 +5737,14 @@
     </row>
     <row r="82" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C82" s="11"/>
       <c r="D82" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E82" s="1">
         <v>564</v>
@@ -5772,14 +5772,14 @@
     </row>
     <row r="83" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C83" s="11"/>
       <c r="D83" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E83" s="1">
         <v>647</v>
@@ -5807,16 +5807,16 @@
     </row>
     <row r="84" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E84" s="1">
         <v>568</v>
@@ -5844,16 +5844,16 @@
     </row>
     <row r="85" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E85" s="1">
         <v>566</v>
@@ -5881,16 +5881,16 @@
     </row>
     <row r="86" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E86" s="1">
         <v>675</v>
@@ -5918,16 +5918,16 @@
     </row>
     <row r="87" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E87" s="1">
         <v>557</v>
@@ -5955,16 +5955,16 @@
     </row>
     <row r="88" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E88" s="1">
         <v>576</v>
@@ -5992,16 +5992,16 @@
     </row>
     <row r="89" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E89" s="1">
         <v>646</v>
@@ -6029,16 +6029,16 @@
     </row>
     <row r="90" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E90" s="1">
         <v>558</v>
@@ -6066,16 +6066,16 @@
     </row>
     <row r="91" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E91" s="1">
         <v>572</v>
@@ -6103,14 +6103,14 @@
     </row>
     <row r="92" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C92" s="11"/>
       <c r="D92" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E92" s="1">
         <v>596</v>
@@ -6138,16 +6138,16 @@
     </row>
     <row r="93" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E93" s="1">
         <v>79</v>
@@ -6175,16 +6175,16 @@
     </row>
     <row r="94" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E94" s="1">
         <v>58</v>
@@ -6212,14 +6212,14 @@
     </row>
     <row r="95" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C95" s="11"/>
       <c r="D95" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E95" s="1">
         <v>580</v>
@@ -6247,14 +6247,14 @@
     </row>
     <row r="96" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C96" s="11"/>
       <c r="D96" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E96" s="1">
         <v>622</v>
@@ -6282,16 +6282,16 @@
     </row>
     <row r="97" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E97" s="1">
         <v>658</v>
@@ -6319,14 +6319,14 @@
     </row>
     <row r="98" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C98" s="11"/>
       <c r="D98" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E98" s="1">
         <v>563</v>
@@ -6354,16 +6354,16 @@
     </row>
     <row r="99" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E99" s="1">
         <v>628</v>
@@ -6391,16 +6391,16 @@
     </row>
     <row r="100" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E100" s="1">
         <v>618</v>
@@ -6428,16 +6428,16 @@
     </row>
     <row r="101" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E101" s="1">
         <v>80</v>
@@ -6465,14 +6465,14 @@
     </row>
     <row r="102" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C102" s="11"/>
       <c r="D102" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E102" s="1">
         <v>667</v>
@@ -6500,14 +6500,14 @@
     </row>
     <row r="103" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C103" s="11"/>
       <c r="D103" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E103" s="1">
         <v>606</v>
@@ -6535,14 +6535,14 @@
     </row>
     <row r="104" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C104" s="11"/>
       <c r="D104" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E104" s="1">
         <v>665</v>
@@ -6570,14 +6570,14 @@
     </row>
     <row r="105" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C105" s="11"/>
       <c r="D105" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E105" s="1">
         <v>131</v>
@@ -6605,14 +6605,14 @@
     </row>
     <row r="106" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C106" s="11"/>
       <c r="D106" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E106" s="1">
         <v>550</v>
@@ -6640,14 +6640,14 @@
     </row>
     <row r="107" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C107" s="11"/>
       <c r="D107" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E107" s="1">
         <v>666</v>
@@ -6675,16 +6675,16 @@
     </row>
     <row r="108" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E108" s="1">
         <v>602</v>
@@ -6712,16 +6712,16 @@
     </row>
     <row r="109" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E109" s="1">
         <v>603</v>
@@ -6749,14 +6749,14 @@
     </row>
     <row r="110" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C110" s="11"/>
       <c r="D110" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E110" s="1">
         <v>589</v>
@@ -6784,16 +6784,16 @@
     </row>
     <row r="111" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E111" s="1">
         <v>586</v>

</xml_diff>